<commit_message>
Update dummy-spreadsheet, fix and add test
- Add generate_dummy to create dummy-spreadsheet.xlsx
- fix data-format test
- add read-write-read continuity test on dummy
</commit_message>
<xml_diff>
--- a/test/resources/dummy-spreadsheet.xlsx
+++ b/test/resources/dummy-spreadsheet.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>A</t>
   </si>
@@ -33,10 +33,16 @@
     <t>Z</t>
   </si>
   <si>
-    <t>#DIV/0!</t>
-  </si>
-  <si>
-    <t>#N/A</t>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
@@ -198,7 +204,7 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyBorder="true" applyFont="true"/>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="2" fontId="15" fillId="5" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true" applyFont="true"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
@@ -211,13 +217,8 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="10.0" customWidth="true"/>
-    <col min="2" max="2" width="10.0" customWidth="true"/>
-    <col min="3" max="3" width="10.0" customWidth="true"/>
-  </cols>
   <sheetData>
-    <row r="1" ht="16.0" customHeight="true">
+    <row r="1">
       <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
@@ -228,7 +229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="16.0" customHeight="true">
+    <row r="2">
       <c r="A2" t="n" s="4">
         <v>1.0</v>
       </c>
@@ -250,7 +251,7 @@
         <v>2.7183</v>
       </c>
     </row>
-    <row r="4" ht="16.0" customHeight="true">
+    <row r="4">
       <c r="A4" t="n" s="10">
         <v>3.0</v>
       </c>
@@ -261,7 +262,7 @@
         <v>1.4142</v>
       </c>
     </row>
-    <row r="5" ht="16.0" customHeight="true">
+    <row r="5">
       <c r="A5" t="n" s="13">
         <f>SUM(A2:A4)</f>
         <v>6.0</v>
@@ -287,13 +288,8 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="10.0" customWidth="true"/>
-    <col min="2" max="2" width="10.0" customWidth="true"/>
-    <col min="3" max="3" width="10.0" customWidth="true"/>
-  </cols>
   <sheetData>
-    <row r="1" ht="16.0" customHeight="true">
+    <row r="1">
       <c r="A1" t="s" s="16">
         <v>3</v>
       </c>
@@ -304,28 +300,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="16.0" customHeight="true">
-      <c r="A2" t="b" s="16">
+    <row r="2">
+      <c r="A2" t="s" s="16">
         <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C2" t="b" s="16">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s" s="16">
         <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" ht="16.0" customHeight="true">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s" s="16">
         <f>1/0</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s" s="16">
         <f>#N/A</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s" s="16">
         <f>#N/A</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update dummy spreadsheet, fix and add test (#38)
* Add formula as an optional parameter

* Update dummy-spreadsheet, fix and add test

- Add generate_dummy to create dummy-spreadsheet.xlsx
- fix data-format test
- add read-write-read continuity test on dummy

* Moved generate_dummy
</commit_message>
<xml_diff>
--- a/test/resources/dummy-spreadsheet.xlsx
+++ b/test/resources/dummy-spreadsheet.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>A</t>
   </si>
@@ -33,10 +33,16 @@
     <t>Z</t>
   </si>
   <si>
-    <t>#DIV/0!</t>
-  </si>
-  <si>
-    <t>#N/A</t>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
@@ -198,7 +204,7 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyBorder="true" applyFont="true"/>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="2" fontId="15" fillId="5" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true" applyFont="true"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
@@ -211,13 +217,8 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="10.0" customWidth="true"/>
-    <col min="2" max="2" width="10.0" customWidth="true"/>
-    <col min="3" max="3" width="10.0" customWidth="true"/>
-  </cols>
   <sheetData>
-    <row r="1" ht="16.0" customHeight="true">
+    <row r="1">
       <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
@@ -228,7 +229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="16.0" customHeight="true">
+    <row r="2">
       <c r="A2" t="n" s="4">
         <v>1.0</v>
       </c>
@@ -250,7 +251,7 @@
         <v>2.7183</v>
       </c>
     </row>
-    <row r="4" ht="16.0" customHeight="true">
+    <row r="4">
       <c r="A4" t="n" s="10">
         <v>3.0</v>
       </c>
@@ -261,7 +262,7 @@
         <v>1.4142</v>
       </c>
     </row>
-    <row r="5" ht="16.0" customHeight="true">
+    <row r="5">
       <c r="A5" t="n" s="13">
         <f>SUM(A2:A4)</f>
         <v>6.0</v>
@@ -287,13 +288,8 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="10.0" customWidth="true"/>
-    <col min="2" max="2" width="10.0" customWidth="true"/>
-    <col min="3" max="3" width="10.0" customWidth="true"/>
-  </cols>
   <sheetData>
-    <row r="1" ht="16.0" customHeight="true">
+    <row r="1">
       <c r="A1" t="s" s="16">
         <v>3</v>
       </c>
@@ -304,28 +300,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="16.0" customHeight="true">
-      <c r="A2" t="b" s="16">
+    <row r="2">
+      <c r="A2" t="s" s="16">
         <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C2" t="b" s="16">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s" s="16">
         <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" ht="16.0" customHeight="true">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s" s="16">
         <f>1/0</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s" s="16">
         <f>#N/A</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s" s="16">
         <f>#N/A</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>